<commit_message>
Latest cmip6 artefacts generated
</commit_message>
<xml_diff>
--- a/cmip5/mappings/ocean/ocean.component-tree.xlsx
+++ b/cmip5/mappings/ocean/ocean.component-tree.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/esdoc-docs/cmip5/vocab-mappings/ocean/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/esdoc-docs/cmip5/mappings/ocean/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="9100" yWindow="1760" windowWidth="24320" windowHeight="17920"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -27,91 +27,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Table 1</t>
   </si>
   <si>
-    <t>cmip5-label</t>
-  </si>
-  <si>
-    <t>cmip5-metafor-id</t>
-  </si>
-  <si>
-    <t>mapping-qc-status</t>
-  </si>
-  <si>
     <t>Ocean</t>
   </si>
   <si>
     <t>Ocean &gt; Advection</t>
   </si>
   <si>
-    <t>OceanAdvection</t>
-  </si>
-  <si>
     <t>Ocean &gt; Boundary Forcing</t>
   </si>
   <si>
-    <t>OceanBoundaryForcing</t>
-  </si>
-  <si>
     <t>Ocean &gt; Boundary Forcing &gt; Tracers</t>
   </si>
   <si>
-    <t>OceanBoundForcingTracers</t>
-  </si>
-  <si>
     <t>Ocean &gt; Lateral Physics</t>
   </si>
   <si>
-    <t>OceanLateralPhysics</t>
-  </si>
-  <si>
     <t>Ocean &gt; Lateral Physics &gt; Momentum</t>
   </si>
   <si>
-    <t>OceanLateralPhysMomentum</t>
-  </si>
-  <si>
     <t>Ocean &gt; Lateral Physics &gt; Tracers</t>
   </si>
   <si>
-    <t>OceanLateralPhysTracers</t>
-  </si>
-  <si>
     <t>Ocean &gt; Upper &amp; Lower Boundaries</t>
   </si>
   <si>
-    <t>OceanUpAndLowBoundaries</t>
-  </si>
-  <si>
     <t>Ocean &gt; Vertical Physics</t>
   </si>
   <si>
-    <t>OceanVerticalPhysics</t>
-  </si>
-  <si>
     <t>Ocean &gt; Vertical Physics &gt; Interior Mixing</t>
   </si>
   <si>
-    <t>OceanInteriorMixing</t>
-  </si>
-  <si>
     <t>Ocean &gt; Vertical Physics &gt; Mixed Layer</t>
   </si>
   <si>
-    <t>OceanMixedLayer</t>
-  </si>
-  <si>
-    <t>cmip6-id</t>
+    <t>cmip6.ocean</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.advection</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.boundary_forcing</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.boundary_forcing.tracers</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.lateral_physics</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.lateral_physics.momentum</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.lateral_physics.tracers</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.uplow_boundaries</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.vertical_physics</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.vertical_physics.interior_mixing</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.vertical_physics.boundary_layer_mixing</t>
+  </si>
+  <si>
+    <t>CMIP5 component [&gt; process]</t>
+  </si>
+  <si>
+    <t>CMIP6 Specialization ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -125,6 +122,12 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
@@ -149,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -189,70 +192,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
@@ -268,45 +211,24 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1497,176 +1419,124 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV13"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="51.6640625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="24.1640625" style="1" customWidth="1"/>
-    <col min="5" max="256" width="8.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="254" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
+    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7">
-        <v>0</v>
+      <c r="B6" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11">
-        <v>0</v>
+      <c r="B8" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="8" t="s">
+    <row r="9" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11">
-        <v>0</v>
+      <c r="B10" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="s">
+    <row r="11" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11">
-        <v>0</v>
+      <c r="B12" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="8" t="s">
+    <row r="13" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="B13" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>